<commit_message>
added reset, and changed name
</commit_message>
<xml_diff>
--- a/CART dependencies/fault_timeseries.xlsx
+++ b/CART dependencies/fault_timeseries.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\CART3_FAC_paper\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7710FA-BFC3-4DC4-BCA1-73C1E4EE4D12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D197A632-327B-414A-8B41-813A9A8F46FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7F115CDE-135B-8C4E-8434-4861B6DBDAA2}"/>
   </bookViews>
   <sheets>
     <sheet name="dT" sheetId="9" r:id="rId1"/>
     <sheet name="dwHSS" sheetId="8" r:id="rId2"/>
-    <sheet name="power_multiplier" sheetId="5" r:id="rId3"/>
-    <sheet name="genTemp" sheetId="4" r:id="rId4"/>
-    <sheet name="ax" sheetId="10" r:id="rId5"/>
+    <sheet name="reset" sheetId="11" r:id="rId3"/>
+    <sheet name="power_multiplier" sheetId="5" r:id="rId4"/>
+    <sheet name="genTemp" sheetId="4" r:id="rId5"/>
+    <sheet name="ax" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,12 +38,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Time [s]</t>
-  </si>
-  <si>
-    <t>wHSS [rad/s]</t>
   </si>
   <si>
     <t>genTemp [C]</t>
@@ -55,6 +53,12 @@
   </si>
   <si>
     <t>ax [g]</t>
+  </si>
+  <si>
+    <t>dwHSS [rad/s]</t>
+  </si>
+  <si>
+    <t>reset</t>
   </si>
 </sst>
 </file>
@@ -95,12 +99,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46D1CE6-F9D0-4450-8EEF-691C0D1369B2}">
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:B182"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B143"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -428,7 +433,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -444,7 +449,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <f ca="1">B2+RAND()*0.01</f>
+        <v>9.1246614640410548E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +458,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>0</v>
+        <f t="shared" ref="B4:B51" ca="1" si="0">B3+RAND()*0.01</f>
+        <v>1.2150262436334904E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,7 +467,8 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.6148969798473103E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +476,8 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.3667982261808055E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +485,8 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1525543019936368E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +494,8 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.5716085390581326E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -492,7 +503,8 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0117858908210076E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -500,7 +512,8 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.7060477331780808E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +521,8 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5.4945643049201354E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +530,8 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5.5852145927257173E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +539,8 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6.2635468730431229E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +548,8 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7.0450922806138308E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +557,8 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7.3900880356973439E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +566,8 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.1537217639180315E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +575,8 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.5593209565985998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +584,8 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.8235022155246576E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +593,8 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.3063073858063922E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +602,8 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.824749516247247E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +611,8 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10164362125046469</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +620,8 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10441008848491622</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +629,8 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10755950083750367</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +638,8 @@
         <v>23</v>
       </c>
       <c r="B24" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.11014127838825893</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +647,8 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.11445676921150956</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +656,8 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1224806577289704</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +665,8 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12515588817167317</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +674,8 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13233728720962104</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +683,8 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13936741913790107</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +692,8 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14135377165000507</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +701,8 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14631489399500799</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +710,8 @@
         <v>31</v>
       </c>
       <c r="B32" s="3">
-        <v>0</v>
+        <f ca="1">B31+RAND()*0.01</f>
+        <v>0.15142558375746135</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +719,8 @@
         <v>32</v>
       </c>
       <c r="B33" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.15478861786436257</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +728,8 @@
         <v>33</v>
       </c>
       <c r="B34" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.15770377391003068</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +737,8 @@
         <v>34</v>
       </c>
       <c r="B35" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16027108172292881</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +746,8 @@
         <v>35</v>
       </c>
       <c r="B36" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16557829979765309</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,7 +755,8 @@
         <v>36</v>
       </c>
       <c r="B37" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16978707625558093</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +764,8 @@
         <v>37</v>
       </c>
       <c r="B38" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1749000644177845</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +773,8 @@
         <v>38</v>
       </c>
       <c r="B39" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18141517768211937</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,7 +782,8 @@
         <v>39</v>
       </c>
       <c r="B40" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1834356049555195</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -748,7 +791,8 @@
         <v>40</v>
       </c>
       <c r="B41" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18549923442288463</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -756,7 +800,8 @@
         <v>41</v>
       </c>
       <c r="B42" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.19360470180054679</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,7 +809,8 @@
         <v>42</v>
       </c>
       <c r="B43" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.19812767366643264</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,7 +818,8 @@
         <v>43</v>
       </c>
       <c r="B44" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.19990578868208139</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,7 +827,8 @@
         <v>44</v>
       </c>
       <c r="B45" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20965779856504763</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,7 +836,8 @@
         <v>45</v>
       </c>
       <c r="B46" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21091581839651918</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +845,8 @@
         <v>46</v>
       </c>
       <c r="B47" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21126063429632197</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -804,7 +854,8 @@
         <v>47</v>
       </c>
       <c r="B48" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21850623702929037</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +863,8 @@
         <v>48</v>
       </c>
       <c r="B49" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22307625710195955</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,7 +872,8 @@
         <v>49</v>
       </c>
       <c r="B50" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22961977968615302</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +881,8 @@
         <v>50</v>
       </c>
       <c r="B51" s="3">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.23336576040531123</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -836,7 +890,8 @@
         <v>51</v>
       </c>
       <c r="B52" s="3">
-        <v>0</v>
+        <f ca="1">0.25+0.01*RAND()</f>
+        <v>0.25469930166663152</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -844,7 +899,8 @@
         <v>52</v>
       </c>
       <c r="B53" s="3">
-        <v>0</v>
+        <f ca="1">0.255+0.01*RAND()</f>
+        <v>0.26107559187583956</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -852,7 +908,8 @@
         <v>53</v>
       </c>
       <c r="B54" s="3">
-        <v>0</v>
+        <f ca="1">0.26+0.01*RAND()</f>
+        <v>0.26565784625285266</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -860,7 +917,8 @@
         <v>54</v>
       </c>
       <c r="B55" s="3">
-        <v>0</v>
+        <f ca="1">0.265+0.01*RAND()</f>
+        <v>0.26975036785627571</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -868,7 +926,8 @@
         <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>0</v>
+        <f ca="1">0.27+0.01*RAND()</f>
+        <v>0.27949667474808143</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -876,7 +935,8 @@
         <v>56</v>
       </c>
       <c r="B57" s="3">
-        <v>0</v>
+        <f ca="1">0.275+0.01*RAND()</f>
+        <v>0.27578720785703897</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -884,7 +944,8 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>0</v>
+        <f ca="1">0.28+0.01*RAND()</f>
+        <v>0.28661971454613722</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -892,7 +953,8 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>0</v>
+        <f ca="1">0.285+0.01*RAND()</f>
+        <v>0.2869575700219279</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -900,7 +962,8 @@
         <v>59</v>
       </c>
       <c r="B60" s="3">
-        <v>0</v>
+        <f>0.296</f>
+        <v>0.29599999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -908,7 +971,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3">
-        <v>0</v>
+        <v>0.29899999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -916,7 +979,8 @@
         <v>61</v>
       </c>
       <c r="B62" s="3">
-        <v>0</v>
+        <f>0.3</f>
+        <v>0.3</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -924,7 +988,8 @@
         <v>62</v>
       </c>
       <c r="B63" s="3">
-        <v>0</v>
+        <f>0.305</f>
+        <v>0.30499999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -932,7 +997,8 @@
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>0</v>
+        <f ca="1">0.31+0.01*RAND()</f>
+        <v>0.31252827844575221</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -940,7 +1006,8 @@
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>0</v>
+        <f ca="1">0.315+0.01*RAND()</f>
+        <v>0.32144570519776539</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -948,7 +1015,8 @@
         <v>65</v>
       </c>
       <c r="B66" s="3">
-        <v>0</v>
+        <f ca="1">0.32+0.01*RAND()</f>
+        <v>0.32259503965906022</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -956,7 +1024,8 @@
         <v>66</v>
       </c>
       <c r="B67" s="3">
-        <v>0</v>
+        <f ca="1">0.325+0.01*RAND()</f>
+        <v>0.33222914223532096</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -964,7 +1033,8 @@
         <v>67</v>
       </c>
       <c r="B68" s="3">
-        <v>0</v>
+        <f ca="1">0.33+0.01*RAND()</f>
+        <v>0.33792077326794956</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -972,7 +1042,8 @@
         <v>68</v>
       </c>
       <c r="B69" s="3">
-        <v>0</v>
+        <f ca="1">0.335+0.01*RAND()</f>
+        <v>0.33941185600955465</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1630,6 +1701,99 @@
       <c r="B151" s="3">
         <v>0</v>
       </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="3"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="3"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B155" s="3"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="3"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="3"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="3"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="3"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="3"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161" s="3"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" s="3"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" s="3"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="3"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165" s="3"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="3"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="3"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="3"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169" s="3"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B170" s="3"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171" s="3"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172" s="3"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173" s="3"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B174" s="3"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175" s="3"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176" s="3"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177" s="3"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178" s="3"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179" s="3"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180" s="3"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181" s="3"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1640,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E19FCB0-EF65-4C30-8599-006CB262BC2E}">
   <dimension ref="A1:B151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B147"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76:B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1651,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1659,8 +1823,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <f t="shared" ref="B2:B65" ca="1" si="0">0.002*RAND()</f>
-        <v>8.0941436395166801E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1668,8 +1831,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.7093155164436242E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1677,8 +1839,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.8968567981992186E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1686,8 +1847,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.3422865216464797E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1695,8 +1855,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.6513746503769718E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1704,8 +1863,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7536795117055947E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1713,8 +1871,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.5012995003717483E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1722,8 +1879,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2779691338851412E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,8 +1887,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5071572019121453E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,8 +1895,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9838431869564999E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1749,8 +1903,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2533739229908169E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,8 +1911,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3371864905231878E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1767,8 +1919,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9917606795148896E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,8 +1927,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9834439217958759E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1785,8 +1935,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7482191265643649E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1794,8 +1943,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7306766749614821E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1803,8 +1951,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.1135128361310818E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1812,8 +1959,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2556019934852137E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1821,8 +1967,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0884035902633301E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1830,8 +1975,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.0585756352823949E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1839,8 +1983,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7273596318350733E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,8 +1991,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.5774434160735802E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1857,8 +1999,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2813407220172919E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1866,8 +2007,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.3257986080414337E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1875,8 +2015,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2913596891025629E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1884,8 +2023,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.3187757807236474E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1893,8 +2031,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7669127912837886E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1902,8 +2039,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.6895143705564541E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1911,8 +2047,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.200606944885186E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1920,8 +2055,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0688880676688794E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1929,8 +2063,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8556239446065678E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1938,8 +2071,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.6210540178619565E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1947,8 +2079,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9724434602071414E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1956,8 +2087,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.990909636018756E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,8 +2095,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1002931635629208E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,8 +2103,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5912214473523211E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1983,8 +2111,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.0736621695585329E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,8 +2119,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5966415184237265E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2001,8 +2127,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9158319355669268E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2010,8 +2135,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.765023784623244E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2019,8 +2143,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.6846022878271791E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2028,8 +2151,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.2342588069977519E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,8 +2159,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.4920190311680096E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2046,8 +2167,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.6624234281215893E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2055,8 +2175,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.7098545325621491E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,8 +2183,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.393437644597911E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,8 +2191,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.6002206488932336E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2082,8 +2199,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.1170725242360145E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,8 +2207,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9203082476393128E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2100,8 +2215,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.525305812142335E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2109,8 +2223,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9717496055014633E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2118,8 +2231,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.5208435173368839E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2127,8 +2239,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.0302720545876577E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,8 +2247,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7377922668055265E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,8 +2255,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.1569178026438365E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2154,8 +2263,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0828300209427494E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2163,8 +2271,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.7852927228873508E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2172,8 +2279,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.1965836382014595E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2181,8 +2287,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.7716143378896694E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2190,8 +2295,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.4862886651294293E-4</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2199,8 +2303,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9669881652015104E-4</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2208,8 +2311,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.8966277706793727E-3</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2217,8 +2319,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7870795795003359E-4</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2226,8 +2327,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.1204181663080615E-3</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2235,8 +2335,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="4">
-        <f t="shared" ref="B66:B129" ca="1" si="1">0.002*RAND()</f>
-        <v>1.3479963436859952E-3</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2244,8 +2343,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.5411841954303008E-5</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2253,8 +2351,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.3166962922103924E-4</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2262,8 +2359,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1304620707841052E-3</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2271,8 +2367,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1963319522510819E-3</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2280,8 +2375,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8910894341722878E-3</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2289,8 +2383,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3231405296526021E-4</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2298,8 +2391,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.8659539082345262E-4</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2307,8 +2399,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.9452166852302573E-4</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2316,8 +2407,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2040652033171925E-3</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2325,8 +2415,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2416448821726258E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2334,8 +2423,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.7383911121757661E-4</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2343,8 +2431,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8916520670040769E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2352,8 +2439,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0196206766697718E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2361,8 +2447,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.3041609707697945E-4</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2370,8 +2455,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2082428234622472E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2379,8 +2463,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9797081609474842E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2388,8 +2471,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2213464167249999E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2397,8 +2479,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6426229066347435E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2406,8 +2487,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.829350368242155E-4</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2415,8 +2495,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6472122003441583E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2424,8 +2503,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4331587906443895E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2433,8 +2511,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.3509773876805297E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2442,8 +2519,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.8423704738807076E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2451,8 +2527,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.5552013111304712E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2460,8 +2535,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3847131143696727E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2469,8 +2543,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.832593866950107E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,8 +2551,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8095165921313099E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,8 +2559,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1162815648435766E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2496,8 +2567,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.9577115209296904E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2505,8 +2575,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.9303921634222628E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2514,8 +2583,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.210911806005642E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2523,8 +2591,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.539372756306051E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2532,8 +2599,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9219204252189151E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2541,8 +2607,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.349038661671013E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,8 +2615,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.7308551016997758E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2559,8 +2623,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.201151705705817E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2568,8 +2631,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8847209517354208E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2577,8 +2639,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.4681230656136343E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2586,8 +2647,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9543874206907883E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2595,8 +2655,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.732893263068016E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2604,8 +2663,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6042121867363636E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2613,8 +2671,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8532933629798933E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2622,8 +2679,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.8480043950170731E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2631,8 +2687,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.3796715230450517E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,8 +2695,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.450484798767204E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2649,8 +2703,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.3129519911681578E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2658,8 +2711,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.7957660664047288E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2667,8 +2719,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.6799141107493415E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2676,8 +2727,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1053398607630436E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2685,8 +2735,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.7274517662429282E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2694,8 +2743,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9819206977657812E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2703,8 +2751,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.042855443615935E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2712,8 +2759,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.6837478005284312E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2721,8 +2767,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.9993261045801143E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2730,8 +2775,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.0062385480811585E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2739,8 +2783,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.5990924154583652E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2748,8 +2791,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6753764623344627E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2757,8 +2799,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6940522850614892E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2766,8 +2807,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.8075691593593049E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2775,8 +2815,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.7152167468415166E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2784,8 +2823,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.7616175872830049E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2793,8 +2831,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.3401922005632123E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2802,8 +2839,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.978815025097831E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2811,8 +2847,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="4">
-        <f t="shared" ref="B130:B147" ca="1" si="2">0.002*RAND()</f>
-        <v>1.2966567850740403E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2820,8 +2855,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>6.3048893426152254E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2829,8 +2863,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.6000989126594566E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2838,8 +2871,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.1382392189380011E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2847,8 +2879,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>7.719287558716583E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2856,8 +2887,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>9.9131808628027496E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2865,8 +2895,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.4773883473281066E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2874,8 +2903,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.7968384208190487E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2883,8 +2911,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.1954910762265371E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2892,8 +2919,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>8.1367275106778217E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -2901,8 +2927,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.2184567220250178E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -2910,8 +2935,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.5255375405932542E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2919,8 +2943,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>2.0849339432899461E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -2928,8 +2951,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.1837586802376573E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -2937,8 +2959,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.4978166893789703E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2946,8 +2967,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>9.5452620416412249E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -2955,8 +2975,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>6.5077732312039368E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -2964,15 +2983,14 @@
         <v>146</v>
       </c>
       <c r="B147" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>8.8155917946313453E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2980,7 +2998,7 @@
       <c r="A149">
         <v>148</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B149" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2988,7 +3006,7 @@
       <c r="A150">
         <v>149</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2996,7 +3014,7 @@
       <c r="A151">
         <v>150</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3007,6 +3025,1229 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB088C8-6793-4398-9B7B-537ADB5331DA}">
+  <dimension ref="A1:B151"/>
+  <sheetViews>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:B151"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DAA9137-9ED1-B74D-A2BB-CEC10A719ABE}">
   <dimension ref="A1:B152"/>
   <sheetViews>
@@ -3024,7 +4265,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4235,7 +5476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041EA285-3496-1944-BDEA-9A9D83515035}">
   <dimension ref="A1:B153"/>
   <sheetViews>
@@ -4253,7 +5494,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5467,7 +6708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2CB20E-E194-4D5D-9D85-D6A81AA420B5}">
   <dimension ref="A1:B121"/>
   <sheetViews>
@@ -5482,7 +6723,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5491,7 +6732,7 @@
       </c>
       <c r="B2">
         <f ca="1">0.1*RAND()</f>
-        <v>8.4901467581498302E-2</v>
+        <v>4.0129982084318533E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5500,7 +6741,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" ca="1" si="0">0.1*RAND()</f>
-        <v>5.7255989115702847E-3</v>
+        <v>7.113110275022487E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5509,7 +6750,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9593788761519793E-2</v>
+        <v>5.1421758963984036E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5518,7 +6759,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3962780757814942E-2</v>
+        <v>8.1379519441584502E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5527,7 +6768,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1269769300451634E-2</v>
+        <v>9.1227036502772044E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5536,7 +6777,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8622602617458865E-2</v>
+        <v>1.1016736255529836E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5545,7 +6786,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1467147001597821E-2</v>
+        <v>4.8735329267283245E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5554,7 +6795,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4811055422014822E-2</v>
+        <v>1.3885796224168623E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5563,7 +6804,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>7.397696414207254E-2</v>
+        <v>5.6288823464391971E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5572,7 +6813,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7150869637122782E-2</v>
+        <v>5.2132995041679536E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5581,7 +6822,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3345290251064446E-2</v>
+        <v>8.7666577801044476E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5590,7 +6831,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4493357085322333E-2</v>
+        <v>8.2125611802624066E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -5599,7 +6840,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4251846702739945E-2</v>
+        <v>2.734518857590781E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -5608,7 +6849,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5264001922577021E-2</v>
+        <v>9.7083715965471981E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5617,7 +6858,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7229270217742345E-2</v>
+        <v>8.0595664770407735E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -5626,7 +6867,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5156262621020143E-2</v>
+        <v>8.1410461478929635E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -5635,7 +6876,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8106271044907327E-2</v>
+        <v>3.1668305295364798E-4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5644,7 +6885,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3001540135439219E-2</v>
+        <v>5.6793656559163568E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -5653,7 +6894,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>6.154645540112013E-2</v>
+        <v>4.8177243311981359E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5662,7 +6903,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1969407902664465E-2</v>
+        <v>5.2097495888978607E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -5671,7 +6912,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3428429151837453E-2</v>
+        <v>2.325375708535107E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -5680,7 +6921,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4618317283422707E-2</v>
+        <v>4.3975361401829727E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5689,7 +6930,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9688294966388388E-2</v>
+        <v>1.7685346791946933E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5698,7 +6939,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4143697672449344E-2</v>
+        <v>5.1004051151281926E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -5707,7 +6948,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3887522014067324E-2</v>
+        <v>3.9275057320254395E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -5716,7 +6957,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0020749340307654E-2</v>
+        <v>7.0150572158230576E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5725,7 +6966,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4059070752822463E-2</v>
+        <v>2.3806930398137239E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -5734,7 +6975,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6043842874701353E-2</v>
+        <v>3.1439524373942228E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -5743,7 +6984,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1568090573644568E-2</v>
+        <v>7.4792336559442743E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -5752,7 +6993,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7704816579654465E-2</v>
+        <v>9.6645308995820967E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -5761,7 +7002,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7870785316900727E-2</v>
+        <v>5.8361088705769809E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -5770,7 +7011,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>3.156359799342312E-2</v>
+        <v>2.8742046059563854E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -5779,7 +7020,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>7.491181581108175E-2</v>
+        <v>3.0801027004518412E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -5788,7 +7029,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8023948496268715E-2</v>
+        <v>9.4727092842340779E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -5797,7 +7038,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9935578848320341E-3</v>
+        <v>8.2601279575824499E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -5806,7 +7047,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1583237618006167E-2</v>
+        <v>7.5001797910335621E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -5815,7 +7056,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8982091691739817E-2</v>
+        <v>7.9487664234690919E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -5824,7 +7065,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>8.935219207147474E-2</v>
+        <v>9.7193601425112297E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -5833,7 +7074,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1508606222596569E-2</v>
+        <v>4.266391860331116E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -5842,7 +7083,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0988272329752412E-2</v>
+        <v>5.2960908570373416E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -5851,7 +7092,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4194850124150746E-4</v>
+        <v>8.2426736056983863E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -5860,7 +7101,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6468121888639778E-2</v>
+        <v>8.241953684406006E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -5869,7 +7110,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5140607643196264E-2</v>
+        <v>9.0137244221393853E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -5878,7 +7119,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7832966860204156E-2</v>
+        <v>1.789303783301829E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -5887,7 +7128,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5065153625302438E-3</v>
+        <v>1.5555431025448286E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -5896,7 +7137,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3540773445353296E-2</v>
+        <v>4.593221024467236E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -5905,7 +7146,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5663464141784069E-2</v>
+        <v>7.4694663645726675E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -5914,7 +7155,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>7.2180647584415045E-2</v>
+        <v>7.7336824867865861E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -5923,7 +7164,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3114770435790802E-2</v>
+        <v>2.0449744398164806E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -5932,7 +7173,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4825558310917953E-2</v>
+        <v>2.5597614031796379E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -5941,7 +7182,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5911093490890572E-2</v>
+        <v>4.5654295592401008E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -5950,7 +7191,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4141659362426162E-2</v>
+        <v>5.2378102365147174E-3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -5959,7 +7200,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7249631495476713E-2</v>
+        <v>6.6550979929400848E-3</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -5968,7 +7209,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6517183550812098E-2</v>
+        <v>3.3174605063302945E-3</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -5977,7 +7218,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9565285050908151E-2</v>
+        <v>3.2925413068097258E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -5986,7 +7227,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2940419340316699E-2</v>
+        <v>1.8597144200775718E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -5995,7 +7236,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1654683516128451E-2</v>
+        <v>4.06644168989767E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -6004,7 +7245,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>8.286076777057072E-2</v>
+        <v>5.7409533737086432E-2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -6013,7 +7254,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7653803402932436E-2</v>
+        <v>5.861329051992116E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -6022,7 +7263,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9692339604047844E-2</v>
+        <v>2.5538143873834785E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -6031,7 +7272,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="0"/>
-        <v>7.2727011455856833E-2</v>
+        <v>4.5603217915710259E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -6040,7 +7281,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4128194132866453E-2</v>
+        <v>6.9698120828231555E-2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -6049,7 +7290,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1552990695815299E-2</v>
+        <v>6.4998475377007106E-2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -6058,7 +7299,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="0"/>
-        <v>4.325971098099636E-2</v>
+        <v>3.4938894586378291E-2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -6067,7 +7308,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4434407474111084E-2</v>
+        <v>5.4459179918629988E-2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -6076,7 +7317,7 @@
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B121" ca="1" si="1">0.1*RAND()</f>
-        <v>8.1130437993127955E-2</v>
+        <v>7.3096628447738718E-2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -6085,7 +7326,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2537260328268258E-2</v>
+        <v>2.5950358929992992E-2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -6094,7 +7335,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1974053131504105E-2</v>
+        <v>9.7749187034624152E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -6103,7 +7344,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0060218464376747E-2</v>
+        <v>1.0021154071185635E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -6112,7 +7353,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1964314291880529E-2</v>
+        <v>2.7737863311121425E-2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -6121,7 +7362,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5462002192014021E-3</v>
+        <v>5.3875400888207026E-2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -6130,7 +7371,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4556528620044337E-2</v>
+        <v>6.5183510817102289E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -6139,7 +7380,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7983843434462352E-2</v>
+        <v>5.7071110891338539E-2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -6148,7 +7389,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3415794162615098E-2</v>
+        <v>1.9427003514442501E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -6157,7 +7398,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0797983671753782E-2</v>
+        <v>2.3813465141969348E-2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -6166,7 +7407,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>4.459635471834123E-3</v>
+        <v>5.7125149861664837E-2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -6175,7 +7416,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6044804226824717E-2</v>
+        <v>6.3899748300078024E-2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -6184,7 +7425,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="1"/>
-        <v>9.195840350978475E-2</v>
+        <v>5.8365096356033465E-2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -6193,7 +7434,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9924081925709611E-3</v>
+        <v>1.7756800040557353E-3</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -6202,7 +7443,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5087040693580738E-2</v>
+        <v>2.3282652085163547E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -6211,7 +7452,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9194572359892955E-2</v>
+        <v>3.0871618619603681E-2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -6220,7 +7461,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5473079334896757E-2</v>
+        <v>3.9250336228981914E-2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -6229,7 +7470,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="1"/>
-        <v>7.076513229175127E-2</v>
+        <v>6.8256602276941622E-2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -6238,7 +7479,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8342795731547967E-2</v>
+        <v>7.8451406020913342E-2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -6247,7 +7488,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5191816183148509E-2</v>
+        <v>2.7797124475828952E-2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -6256,7 +7497,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8744924856277134E-2</v>
+        <v>1.9270054932326031E-2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -6265,7 +7506,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0461657026219246E-2</v>
+        <v>6.2262993056533524E-2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -6274,7 +7515,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7345616043630943E-2</v>
+        <v>5.95117771480312E-2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -6283,7 +7524,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="1"/>
-        <v>4.655905707728674E-2</v>
+        <v>2.2296928059962431E-2</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -6292,7 +7533,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6929011576557849E-2</v>
+        <v>3.4142081792203814E-2</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -6301,7 +7542,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="1"/>
-        <v>6.9391030016550989E-2</v>
+        <v>9.5370851355767353E-2</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -6310,7 +7551,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="1"/>
-        <v>5.378299514591927E-2</v>
+        <v>5.9471271454378033E-3</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -6319,7 +7560,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="1"/>
-        <v>6.398756358064904E-2</v>
+        <v>6.6391693647829514E-2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -6328,7 +7569,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1794117384413087E-2</v>
+        <v>3.6827335968943997E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -6337,7 +7578,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1975881696865197E-2</v>
+        <v>5.9862356670866257E-2</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -6346,7 +7587,7 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8799083405769648E-2</v>
+        <v>8.3540557972571206E-2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -6355,7 +7596,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1849135101479563E-2</v>
+        <v>7.5660056947826852E-3</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -6364,7 +7605,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="1"/>
-        <v>1.312604546784394E-2</v>
+        <v>7.0327170280059234E-2</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -6373,7 +7614,7 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7415086347341049E-2</v>
+        <v>7.6458397531981373E-2</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -6382,7 +7623,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5063088909434376E-2</v>
+        <v>5.9679087947901367E-2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -6391,7 +7632,7 @@
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2598906278699574E-2</v>
+        <v>8.6413462653661899E-2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -6400,7 +7641,7 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3742149500200792E-2</v>
+        <v>2.0865457968780657E-2</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -6409,7 +7650,7 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4294422058556998E-2</v>
+        <v>6.0716021335610659E-2</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -6418,7 +7659,7 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4870871635489794E-2</v>
+        <v>1.6280557820718567E-2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -6427,7 +7668,7 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0960773263044725E-2</v>
+        <v>7.4154407142821052E-2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -6436,7 +7677,7 @@
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="1"/>
-        <v>4.766133262837198E-2</v>
+        <v>6.0697977711570421E-2</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -6445,7 +7686,7 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8808804734117647E-2</v>
+        <v>2.0688974411607199E-2</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -6454,7 +7695,7 @@
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0765655140657014E-2</v>
+        <v>9.6425189737549849E-2</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -6463,7 +7704,7 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0699046990861357E-2</v>
+        <v>5.3471163652746845E-2</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -6472,7 +7713,7 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6359359031973684E-2</v>
+        <v>4.4087079686855629E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -6481,7 +7722,7 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="1"/>
-        <v>1.295303071457321E-2</v>
+        <v>7.3537824783320146E-2</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -6490,7 +7731,7 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="1"/>
-        <v>7.978978276607035E-2</v>
+        <v>7.2413904085176783E-3</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -6499,7 +7740,7 @@
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="1"/>
-        <v>2.80229025003816E-2</v>
+        <v>9.9484547718843325E-2</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -6508,7 +7749,7 @@
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="1"/>
-        <v>8.5369709602830329E-2</v>
+        <v>9.2365525796591783E-2</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -6517,7 +7758,7 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2222267323755682E-2</v>
+        <v>6.2373189410461799E-2</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -6526,7 +7767,7 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8368963476331406E-2</v>
+        <v>2.0685752068068442E-3</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -6535,7 +7776,7 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5227608607049332E-2</v>
+        <v>3.8196869111771406E-2</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -6544,7 +7785,7 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0743592671501384E-2</v>
+        <v>2.265622499519231E-2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -6553,7 +7794,7 @@
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7940507791090726E-3</v>
+        <v>2.3012677556616758E-2</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -6562,7 +7803,7 @@
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="1"/>
-        <v>5.228881093070073E-2</v>
+        <v>4.6750625344888885E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>